<commit_message>
Heperlink of imp topics added
</commit_message>
<xml_diff>
--- a/Interview Preparation combat.xlsx
+++ b/Interview Preparation combat.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aditya1.Aggarwal\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aditya1.Aggarwal\Documents\Preparation Material Job\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t>C++</t>
   </si>
@@ -453,7 +453,10 @@
     <t xml:space="preserve">Recursion </t>
   </si>
   <si>
-    <t>concept By :- love babbar and question by :-  nishant chhahar</t>
+    <t>Lexicographical alphabets</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> youtube :- code in 10 (nishant chhahar)</t>
   </si>
 </sst>
 </file>
@@ -811,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,7 +905,7 @@
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
       <c r="J7" t="s">
@@ -919,7 +922,7 @@
       <c r="A8" t="s">
         <v>111</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="4" t="s">
         <v>48</v>
       </c>
       <c r="P8" t="s">
@@ -930,7 +933,7 @@
       <c r="A9" t="s">
         <v>23</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="4" t="s">
         <v>49</v>
       </c>
       <c r="P9" t="s">
@@ -946,7 +949,7 @@
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
       <c r="J11" t="s">
@@ -965,7 +968,7 @@
       <c r="A13" t="s">
         <v>115</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="4" t="s">
         <v>62</v>
       </c>
     </row>
@@ -981,7 +984,7 @@
       <c r="A15" t="s">
         <v>114</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="4" t="s">
         <v>78</v>
       </c>
       <c r="W15" s="3" t="s">
@@ -1112,7 +1115,7 @@
         <v>119</v>
       </c>
       <c r="D26" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K26" t="s">
         <v>69</v>
@@ -1135,6 +1138,9 @@
       </c>
       <c r="K28" t="s">
         <v>35</v>
+      </c>
+      <c r="W28" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
@@ -1274,12 +1280,18 @@
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" location="explain-hoisting"/>
     <hyperlink ref="J3" r:id="rId2" location="explain-closures"/>
-    <hyperlink ref="J4" r:id="rId3" location="difference-between-var-and-let-keyword-in-javascript"/>
+    <hyperlink ref="J4" r:id="rId3" location="differences-between-declaring-variables-using-var-let-and-const"/>
     <hyperlink ref="J18" r:id="rId4" location="difference-between-and-operators"/>
     <hyperlink ref="J5" r:id="rId5" location="memoization"/>
     <hyperlink ref="J6" r:id="rId6" location="dom"/>
+    <hyperlink ref="J13" r:id="rId7" location="call-apply-and-bind-methods"/>
+    <hyperlink ref="J9" r:id="rId8" location="different-data-types-present-in-javascript"/>
+    <hyperlink ref="J15" r:id="rId9" location="arrow-functions"/>
+    <hyperlink ref="J8" r:id="rId10" location="rest-parameter-and-spread-operator"/>
+    <hyperlink ref="A11" r:id="rId11" location="inline-function"/>
+    <hyperlink ref="A7" r:id="rId12" location="abstract-class"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add ans go hr type ques and hover the red arrow for ans
</commit_message>
<xml_diff>
--- a/Interview Preparation combat.xlsx
+++ b/Interview Preparation combat.xlsx
@@ -23,6 +23,116 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Aditya1 Aggarwal</author>
+  </authors>
+  <commentList>
+    <comment ref="X2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Aditya1 Aggarwal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ Hi. I am Mohit Gautam. I have completed my Engineering from Gautam Buddha University, specializing in Information Technology recently. During my time in college, I got good grades.
+ I have always been interested in Web Development and have done several projects based on React and Django. I have assisted my teammates on several occasions to finish their projects.
+ I am a person with critical thinking skills and have the ability to turn a regular project into something innovative. My final year major project is based on Ecommerce web application using Html,css ,javascript in frontend and Python and Django as backened. A web application can be develop using nodejs which is one of the hot using framework of javascript, but we chose to make the project innovative using an django in in as backened which is used by many companies write know. I have good circuitry knowledge.
+ I always put quality on top of anything, and whatever projects I made were real-life projects. I also possess good communication skills and would like to improve my skills by working in your company.
+I love learning new things and always have been that person who has high enthusiast in new technology in computer science field .</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Aditya1 Aggarwal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+I am a self-motivated and very open-minded person who can learn very fast. Looking at the job description and my experience in the field of web development, I am confident that I am very much suitable for this role. I enjoy solving problems and I am a great team player. I also believe that my values are aligned with this company’s values. I think this position will support my interest and also give me interesting and exciting opportunities to contribute to the growth of this organization. I am very much excited about this opportunity</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Aditya1 Aggarwal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+I think one of my greatest strengths is that I am a great team player. I am also a self-motivated and quick learning individual. Whatever task that I set to do, I always give my best and complete it diligently well in advance. My weakness would be that I am learning to master people skills while meeting new individuals. I get nervous while talking to new people. I have been working on this for quite a long time and I can say with utmost confidence that I have come a long way.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Aditya1 Aggarwal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Over 5 years, I would love to utilize all the opportunities that this company provides me to learn by utilizing the internal and external training programs. My ultimate career goal is to become a Technology Architect and hence I would look forward to developing various products that represent the vision of this company and be a part of making a difference along with quickening my journey of becoming a Tech Architect</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
@@ -38,9 +148,6 @@
     <t>Binary Search</t>
   </si>
   <si>
-    <t>Maximum Sum sub Array</t>
-  </si>
-  <si>
     <t>first bad version</t>
   </si>
   <si>
@@ -51,9 +158,6 @@
   </si>
   <si>
     <t xml:space="preserve">XOR </t>
-  </si>
-  <si>
-    <t>,Book Allocation Problem</t>
   </si>
   <si>
     <t>String</t>
@@ -238,9 +342,6 @@
   </si>
   <si>
     <t>Tell me about yourself</t>
-  </si>
-  <si>
-    <t>Why do we hire you</t>
   </si>
   <si>
     <t xml:space="preserve">Attribute and types of attribute </t>
@@ -458,12 +559,21 @@
   <si>
     <t xml:space="preserve"> youtube :- code in 10 (nishant chhahar)</t>
   </si>
+  <si>
+    <t xml:space="preserve">,            </t>
+  </si>
+  <si>
+    <t>Maximum Sum sub Array, Book Allocation Problem</t>
+  </si>
+  <si>
+    <t>Why should we hire you</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -502,6 +612,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -811,11 +934,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,200 +948,200 @@
         <v>0</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="X2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="P3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="X3" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P4" t="s">
+        <v>38</v>
+      </c>
+      <c r="X4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="P5" t="s">
         <v>40</v>
       </c>
-      <c r="X4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="P5" t="s">
-        <v>42</v>
-      </c>
       <c r="X5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="X6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="X7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="P8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>114</v>
+      <c r="A15" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="W15" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="W16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J17" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="W17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="J18" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="W18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
@@ -1026,15 +1149,15 @@
         <v>1</v>
       </c>
       <c r="W19" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="W20" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
@@ -1042,16 +1165,16 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>4</v>
+        <v>120</v>
       </c>
       <c r="F21" t="s">
-        <v>9</v>
+        <v>119</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="W21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
@@ -1059,221 +1182,221 @@
         <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="W22" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
         <v>6</v>
       </c>
-      <c r="D23" t="s">
-        <v>7</v>
-      </c>
       <c r="K23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="W23" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="W24" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D25" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="W25" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="K26" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="W26" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="K27" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="W27" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="W28" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K29" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="K31" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U34" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K35" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="U35" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K36" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="U36" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K37" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="U37" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U38" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K39" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U39" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="U40" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="U41" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="U42" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="L44" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="L45" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1290,8 +1413,11 @@
     <hyperlink ref="J8" r:id="rId10" location="rest-parameter-and-spread-operator"/>
     <hyperlink ref="A11" r:id="rId11" location="inline-function"/>
     <hyperlink ref="A7" r:id="rId12" location="abstract-class"/>
+    <hyperlink ref="A15" r:id="rId13"/>
+    <hyperlink ref="A5" r:id="rId14" location="polymorphism-in-c++"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
+  <legacyDrawing r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add more link and comment for answer hover it
</commit_message>
<xml_diff>
--- a/Interview Preparation combat.xlsx
+++ b/Interview Preparation combat.xlsx
@@ -29,6 +29,30 @@
     <author>Aditya1 Aggarwal</author>
   </authors>
   <commentList>
+    <comment ref="A2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Aditya1 Aggarwal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+static keyword is used to reserved copy of a variable in program means if any variable create static then a copy of variable will remain in ram can change unitl the whole execution of prgram is not done even if function call end it has  reserved memory and has a property that it will create only one time fror one object or for more.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="X2" authorId="0" shapeId="0">
       <text>
         <r>
@@ -937,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Z9" sqref="Z9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,7 +996,7 @@
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>41</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -1031,7 +1055,7 @@
       <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="4" t="s">
         <v>45</v>
       </c>
       <c r="P7" t="s">
@@ -1042,7 +1066,7 @@
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
         <v>108</v>
       </c>
       <c r="J8" s="4" t="s">
@@ -1067,7 +1091,7 @@
       <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="4" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1075,7 +1099,7 @@
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1415,9 +1439,14 @@
     <hyperlink ref="A7" r:id="rId12" location="abstract-class"/>
     <hyperlink ref="A15" r:id="rId13"/>
     <hyperlink ref="A5" r:id="rId14" location="polymorphism-in-c++"/>
+    <hyperlink ref="J7" r:id="rId15"/>
+    <hyperlink ref="J10" r:id="rId16"/>
+    <hyperlink ref="J11" r:id="rId17"/>
+    <hyperlink ref="A3" r:id="rId18"/>
+    <hyperlink ref="A8" r:id="rId19" location="virtual-function-and-pure-virtual-function"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
-  <legacyDrawing r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
+  <legacyDrawing r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>